<commit_message>
update and subjects added
</commit_message>
<xml_diff>
--- a/ExperimentFolder_v23.9.19/Paradigma/Protocol/protocol.xlsx
+++ b/ExperimentFolder_v23.9.19/Paradigma/Protocol/protocol.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="34">
   <si>
     <t>Subject ID</t>
   </si>
@@ -76,6 +76,48 @@
   </si>
   <si>
     <t>nothing</t>
+  </si>
+  <si>
+    <t>fw</t>
+  </si>
+  <si>
+    <t>lp</t>
+  </si>
+  <si>
+    <t>mb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m </t>
+  </si>
+  <si>
+    <t>mch</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>pg</t>
+  </si>
+  <si>
+    <t>occasionally</t>
+  </si>
+  <si>
+    <t>ap</t>
+  </si>
+  <si>
+    <t>tinnitus (re/li) higher than usual</t>
+  </si>
+  <si>
+    <t>lila -&gt; violet</t>
+  </si>
+  <si>
+    <t>lb</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>bad mood</t>
   </si>
 </sst>
 </file>
@@ -414,23 +456,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
-    <col min="2" max="2" width="4.44140625" customWidth="1"/>
-    <col min="3" max="3" width="4.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="46.44140625" customWidth="1"/>
-    <col min="6" max="6" width="53.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" customWidth="1"/>
+    <col min="6" max="6" width="53.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.140625" customWidth="1"/>
+    <col min="9" max="9" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -517,6 +559,238 @@
         <v>19</v>
       </c>
       <c r="I3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" t="s">
         <v>19</v>
       </c>
     </row>
@@ -532,7 +806,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -544,7 +818,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>